<commit_message>
Added dataset discription that is heavily biased toward male-heterogametic species
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B6C5DE-C7C4-41AD-975B-26A21C577C98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C91C308-FE1C-4AAE-885D-FC97B26FA479}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18480" windowHeight="11020" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18480" windowHeight="11020" tabRatio="997" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
@@ -2945,12 +2945,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
     <t>Allopatry</t>
   </si>
   <si>
@@ -3012,6 +3006,12 @@
   <si>
     <t>NA</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -3972,11 +3972,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR557"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="16"/>
@@ -10736,12 +10736,12 @@
       <c r="S64" s="20"/>
       <c r="T64" s="20"/>
       <c r="U64" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V64" s="20"/>
       <c r="W64" s="20"/>
       <c r="X64" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y64" s="20"/>
       <c r="Z64" s="20"/>
@@ -10833,12 +10833,12 @@
       <c r="S65" s="20"/>
       <c r="T65" s="20"/>
       <c r="U65" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V65" s="20"/>
       <c r="W65" s="20"/>
       <c r="X65" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y65" s="20"/>
       <c r="Z65" s="20"/>
@@ -10930,12 +10930,12 @@
       <c r="S66" s="20"/>
       <c r="T66" s="20"/>
       <c r="U66" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V66" s="20"/>
       <c r="W66" s="20"/>
       <c r="X66" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y66" s="20"/>
       <c r="Z66" s="20"/>
@@ -11027,12 +11027,12 @@
       <c r="S67" s="20"/>
       <c r="T67" s="20"/>
       <c r="U67" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V67" s="20"/>
       <c r="W67" s="20"/>
       <c r="X67" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y67" s="20"/>
       <c r="Z67" s="20"/>
@@ -11124,12 +11124,12 @@
       <c r="S68" s="20"/>
       <c r="T68" s="20"/>
       <c r="U68" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V68" s="20"/>
       <c r="W68" s="20"/>
       <c r="X68" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y68" s="20"/>
       <c r="Z68" s="20"/>
@@ -11221,12 +11221,12 @@
       <c r="S69" s="20"/>
       <c r="T69" s="20"/>
       <c r="U69" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="V69" s="20"/>
       <c r="W69" s="20"/>
       <c r="X69" s="28" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Y69" s="20"/>
       <c r="Z69" s="20"/>
@@ -49852,7 +49852,7 @@
         <v>26</v>
       </c>
       <c r="N494" s="20" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="O494" s="28"/>
       <c r="P494" s="20">
@@ -49954,7 +49954,7 @@
         <v>26</v>
       </c>
       <c r="N495" s="20" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="O495" s="28"/>
       <c r="P495" s="20">
@@ -50057,7 +50057,7 @@
         <v>26</v>
       </c>
       <c r="N496" s="20" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="O496" s="28"/>
       <c r="P496" s="20">
@@ -50159,7 +50159,7 @@
         <v>26</v>
       </c>
       <c r="N497" s="20" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="O497" s="28"/>
       <c r="P497" s="20">
@@ -61987,10 +61987,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5C8A46-EA2B-4375-A470-1D2BA981D131}">
   <dimension ref="A1:Z571"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="16.5"/>
@@ -62029,7 +62029,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>727</v>
@@ -62038,10 +62038,10 @@
         <v>636</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J1" s="21" t="s">
         <v>754</v>
@@ -62101,7 +62101,7 @@
         <v>433</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>728</v>
@@ -62110,13 +62110,13 @@
         <v>638</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>26</v>
@@ -62164,7 +62164,7 @@
         <v>438</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F3" s="45" t="s">
         <v>728</v>
@@ -62173,13 +62173,13 @@
         <v>638</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K3" s="25" t="s">
         <v>26</v>
@@ -62227,7 +62227,7 @@
         <v>750</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F4" s="45" t="s">
         <v>728</v>
@@ -62236,13 +62236,13 @@
         <v>638</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>26</v>
@@ -62287,7 +62287,7 @@
         <v>751</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F5" s="45" t="s">
         <v>728</v>
@@ -62296,13 +62296,13 @@
         <v>638</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>26</v>
@@ -62347,7 +62347,7 @@
         <v>441</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>728</v>
@@ -62356,13 +62356,13 @@
         <v>638</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>26</v>
@@ -62407,7 +62407,7 @@
         <v>439</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F7" s="45" t="s">
         <v>728</v>
@@ -62416,13 +62416,13 @@
         <v>638</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I7" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K7" s="25" t="s">
         <v>26</v>
@@ -62471,7 +62471,7 @@
         <v>Agrotis_ipsilon_Agrotis_segetum</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F8" s="45" t="s">
         <v>728</v>
@@ -62480,13 +62480,13 @@
         <v>643</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I8" s="32" t="s">
         <v>648</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
       <c r="K8" s="34">
         <v>7.5999999999999998E-2</v>
@@ -62541,7 +62541,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F9" s="45" t="s">
         <v>728</v>
@@ -62550,13 +62550,13 @@
         <v>638</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L9" s="40">
         <v>5.0999999999999997E-2</v>
@@ -62600,7 +62600,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F10" s="45" t="s">
         <v>728</v>
@@ -62609,13 +62609,13 @@
         <v>638</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K10" s="25" t="s">
         <v>26</v>
@@ -62668,7 +62668,7 @@
         <v>70</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F11" s="45" t="s">
         <v>728</v>
@@ -62677,13 +62677,13 @@
         <v>638</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K11" s="25" t="s">
         <v>26</v>
@@ -62736,7 +62736,7 @@
         <v>722</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F12" s="45" t="s">
         <v>728</v>
@@ -62745,13 +62745,13 @@
         <v>638</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K12" s="25" t="s">
         <v>26</v>
@@ -62805,7 +62805,7 @@
         <v>Carabus_iwawakianus_Carabus_maiyasanus</v>
       </c>
       <c r="E13" s="46" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F13" s="45" t="s">
         <v>728</v>
@@ -62814,13 +62814,13 @@
         <v>737</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>738</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>26</v>
@@ -62855,7 +62855,7 @@
         <v>399</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F14" s="45" t="s">
         <v>728</v>
@@ -62864,13 +62864,13 @@
         <v>638</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I14" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L14" s="40">
         <v>3.496</v>
@@ -62912,7 +62912,7 @@
         <v>Chorthippus_biguttulus_Chorthippus_brunneus</v>
       </c>
       <c r="E15" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F15" s="45" t="s">
         <v>728</v>
@@ -62921,13 +62921,13 @@
         <v>642</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K15" s="34">
         <v>7.0000000000000001E-3</v>
@@ -62969,7 +62969,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="21" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>601</v>
@@ -62983,7 +62983,7 @@
         <v>Chrysoperla_johnsoni_Chrysoperla_plorabunda</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F16" s="45" t="s">
         <v>728</v>
@@ -62992,13 +62992,13 @@
         <v>644</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K16" s="25" t="s">
         <v>26</v>
@@ -63049,7 +63049,7 @@
         <v>Drosophila_biauraria_Drosophila_subauraria</v>
       </c>
       <c r="E17" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F17" s="45" t="s">
         <v>728</v>
@@ -63058,13 +63058,13 @@
         <v>638</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I17" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K17" s="25" t="s">
         <v>26</v>
@@ -63109,7 +63109,7 @@
         <v>Drosophila_borealis_Drosophila_virilis</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F18" s="45" t="s">
         <v>728</v>
@@ -63118,13 +63118,13 @@
         <v>638</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K18" s="25" t="s">
         <v>26</v>
@@ -63172,7 +63172,7 @@
         <v>Drosophila_buzzatii_Drosophila_koepferae</v>
       </c>
       <c r="E19" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F19" s="45" t="s">
         <v>728</v>
@@ -63181,13 +63181,13 @@
         <v>638</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L19" s="40">
         <v>1.0529999999999999</v>
@@ -63229,7 +63229,7 @@
         <v>Drosophila_flavomontana_Drosophila_lacicola</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F20" s="45" t="s">
         <v>728</v>
@@ -63238,13 +63238,13 @@
         <v>638</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K20" s="25" t="s">
         <v>26</v>
@@ -63296,7 +63296,7 @@
         <v>Drosophila_flavomontana_Drosophila_littoralis</v>
       </c>
       <c r="E21" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F21" s="45" t="s">
         <v>730</v>
@@ -63305,13 +63305,13 @@
         <v>638</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I21" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K21" s="25" t="s">
         <v>26</v>
@@ -63356,7 +63356,7 @@
         <v>Drosophila_flavomontana_Drosophila_montana</v>
       </c>
       <c r="E22" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F22" s="45" t="s">
         <v>730</v>
@@ -63365,13 +63365,13 @@
         <v>638</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I22" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K22" s="25" t="s">
         <v>26</v>
@@ -63416,7 +63416,7 @@
         <v>Drosophila_flavomontana_Drosophila_virilis</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F23" s="45" t="s">
         <v>728</v>
@@ -63425,13 +63425,13 @@
         <v>638</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I23" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K23" s="34" t="s">
         <v>26</v>
@@ -63480,7 +63480,7 @@
         <v>Drosophila_heteroneura_Drosophila_silvestris</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F24" s="45" t="s">
         <v>733</v>
@@ -63489,13 +63489,13 @@
         <v>638</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>26</v>
@@ -63549,7 +63549,7 @@
         <v>Drosophila_kanekoi_Drosophila_virilis</v>
       </c>
       <c r="E25" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F25" s="45" t="s">
         <v>728</v>
@@ -63558,13 +63558,13 @@
         <v>638</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K25" s="25" t="s">
         <v>26</v>
@@ -63612,7 +63612,7 @@
         <v>Drosophila_littoralis_Drosophila_virilis</v>
       </c>
       <c r="E26" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F26" s="45" t="s">
         <v>728</v>
@@ -63621,13 +63621,13 @@
         <v>638</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K26" s="34">
         <v>0.128</v>
@@ -63680,7 +63680,7 @@
         <v>Drosophila_lummei_Drosophila_virilis</v>
       </c>
       <c r="E27" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F27" s="45" t="s">
         <v>728</v>
@@ -63689,13 +63689,13 @@
         <v>638</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I27" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K27" s="25">
         <v>0.06</v>
@@ -63749,7 +63749,7 @@
         <v>Drosophila_montana_Drosophila_virilis</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F28" s="45" t="s">
         <v>728</v>
@@ -63758,13 +63758,13 @@
         <v>638</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I28" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K28" s="34" t="s">
         <v>26</v>
@@ -63813,7 +63813,7 @@
         <v>Drosophila_persimilis_Drosophila_pseudoobscura</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F29" s="45" t="s">
         <v>728</v>
@@ -63822,13 +63822,13 @@
         <v>638</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I29" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K29" s="25">
         <v>0.89300000000000002</v>
@@ -63862,7 +63862,7 @@
         <v>Drosophila_quadraria_Drosophila_biauraria</v>
       </c>
       <c r="E30" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F30" s="45" t="s">
         <v>728</v>
@@ -63871,13 +63871,13 @@
         <v>638</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K30" s="25" t="s">
         <v>26</v>
@@ -63922,7 +63922,7 @@
         <v>Drosophila_quadraria_Drosophila_subauraria</v>
       </c>
       <c r="E31" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F31" s="45" t="s">
         <v>728</v>
@@ -63931,13 +63931,13 @@
         <v>638</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K31" s="25" t="s">
         <v>26</v>
@@ -63982,7 +63982,7 @@
         <v>Drosophila_triauraria_Drosophila_biauraria</v>
       </c>
       <c r="E32" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F32" s="45" t="s">
         <v>728</v>
@@ -63991,13 +63991,13 @@
         <v>638</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I32" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K32" s="25" t="s">
         <v>26</v>
@@ -64042,7 +64042,7 @@
         <v>Drosophila_triauraria_Drosophila_quadraria</v>
       </c>
       <c r="E33" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F33" s="45" t="s">
         <v>728</v>
@@ -64051,13 +64051,13 @@
         <v>638</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I33" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J33" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K33" s="25" t="s">
         <v>26</v>
@@ -64101,7 +64101,7 @@
         <v>723</v>
       </c>
       <c r="E34" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F34" s="45" t="s">
         <v>728</v>
@@ -64110,13 +64110,13 @@
         <v>639</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I34" s="32" t="s">
         <v>652</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
       <c r="K34" s="34">
         <v>1.7999999999999999E-2</v>
@@ -64169,7 +64169,7 @@
         <v>724</v>
       </c>
       <c r="E35" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F35" s="45" t="s">
         <v>728</v>
@@ -64178,13 +64178,13 @@
         <v>639</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I35" s="32" t="s">
         <v>652</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
       <c r="K35" s="34">
         <v>1.7999999999999999E-2</v>
@@ -64237,7 +64237,7 @@
         <v>82</v>
       </c>
       <c r="E36" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F36" s="45" t="s">
         <v>728</v>
@@ -64246,13 +64246,13 @@
         <v>638</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I36" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K36" s="25">
         <v>1.7000000000000001E-2</v>
@@ -64296,7 +64296,7 @@
         <v>76</v>
       </c>
       <c r="E37" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F37" s="45" t="s">
         <v>728</v>
@@ -64305,13 +64305,13 @@
         <v>638</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I37" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K37" s="25">
         <v>1.7000000000000001E-2</v>
@@ -64356,7 +64356,7 @@
         <v>Gryllus_armatus_Gryllus_rubens</v>
       </c>
       <c r="E38" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F38" s="45" t="s">
         <v>730</v>
@@ -64365,13 +64365,13 @@
         <v>642</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I38" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K38" s="34" t="s">
         <v>26</v>
@@ -64422,7 +64422,7 @@
         <v>Gryllus_campestris_Gryllus_rubens</v>
       </c>
       <c r="E39" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F39" s="45" t="s">
         <v>730</v>
@@ -64431,13 +64431,13 @@
         <v>642</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I39" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K39" s="34">
         <v>0.111</v>
@@ -64488,7 +64488,7 @@
         <v>Gryllus_rubens_Gryllus_texensis</v>
       </c>
       <c r="E40" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F40" s="45" t="s">
         <v>728</v>
@@ -64497,13 +64497,13 @@
         <v>642</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I40" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K40" s="25">
         <v>4.0000000000000001E-3</v>
@@ -64556,7 +64556,7 @@
         <v>395</v>
       </c>
       <c r="E41" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F41" s="45" t="s">
         <v>728</v>
@@ -64565,13 +64565,13 @@
         <v>638</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J41" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L41" s="40">
         <v>3.496</v>
@@ -64613,7 +64613,7 @@
         <v>Haplochromis_burtoni_Haplochromis_nubilus</v>
       </c>
       <c r="E42" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F42" s="45" t="s">
         <v>728</v>
@@ -64667,7 +64667,7 @@
         <v>Hyla_chrysoscelis_Hyla_femoralis</v>
       </c>
       <c r="E43" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F43" s="45" t="s">
         <v>728</v>
@@ -64676,13 +64676,13 @@
         <v>637</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="I43" s="32" t="s">
         <v>646</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K43" s="25">
         <v>3.1E-2</v>
@@ -64715,7 +64715,7 @@
         <v>403</v>
       </c>
       <c r="E44" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F44" s="45" t="s">
         <v>728</v>
@@ -64724,13 +64724,13 @@
         <v>642</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I44" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K44" s="25" t="s">
         <v>26</v>
@@ -64774,7 +64774,7 @@
         <v>400</v>
       </c>
       <c r="E45" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F45" s="45" t="s">
         <v>728</v>
@@ -64783,13 +64783,13 @@
         <v>638</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L45" s="40">
         <v>3.496</v>
@@ -64830,7 +64830,7 @@
         <v>401</v>
       </c>
       <c r="E46" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F46" s="45" t="s">
         <v>728</v>
@@ -64839,13 +64839,13 @@
         <v>638</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J46" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L46" s="40">
         <v>3.496</v>
@@ -64886,7 +64886,7 @@
         <v>130</v>
       </c>
       <c r="E47" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F47" s="45" t="s">
         <v>728</v>
@@ -64895,13 +64895,13 @@
         <v>640</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I47" s="32" t="s">
         <v>646</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K47" s="34">
         <v>3.1E-2</v>
@@ -64951,7 +64951,7 @@
         <v>386</v>
       </c>
       <c r="E48" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F48" s="45" t="s">
         <v>728</v>
@@ -64960,13 +64960,13 @@
         <v>640</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="I48" s="32" t="s">
         <v>646</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K48" s="34">
         <v>3.1E-2</v>
@@ -65016,7 +65016,7 @@
         <v>409</v>
       </c>
       <c r="E49" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F49" s="45" t="s">
         <v>728</v>
@@ -65025,13 +65025,13 @@
         <v>642</v>
       </c>
       <c r="H49" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I49" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K49" s="25" t="s">
         <v>26</v>
@@ -65075,7 +65075,7 @@
         <v>86</v>
       </c>
       <c r="E50" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F50" s="45" t="s">
         <v>728</v>
@@ -65084,13 +65084,13 @@
         <v>638</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I50" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J50" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K50" s="25">
         <v>1.7000000000000001E-2</v>
@@ -65134,7 +65134,7 @@
         <v>32</v>
       </c>
       <c r="E51" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F51" s="45" t="s">
         <v>728</v>
@@ -65143,13 +65143,13 @@
         <v>642</v>
       </c>
       <c r="H51" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I51" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K51" s="25" t="s">
         <v>26</v>
@@ -65202,7 +65202,7 @@
         <v>38</v>
       </c>
       <c r="E52" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F52" s="45" t="s">
         <v>728</v>
@@ -65211,13 +65211,13 @@
         <v>642</v>
       </c>
       <c r="H52" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I52" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J52" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K52" s="25" t="s">
         <v>26</v>
@@ -65270,7 +65270,7 @@
         <v>92</v>
       </c>
       <c r="E53" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F53" s="45" t="s">
         <v>728</v>
@@ -65279,13 +65279,13 @@
         <v>638</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I53" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J53" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K53" s="25" t="s">
         <v>26</v>
@@ -65330,7 +65330,7 @@
         <v>Pundamilia_nyererei_Pundamilia_pundamilia</v>
       </c>
       <c r="E54" s="62" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F54" s="45" t="s">
         <v>728</v>
@@ -65389,7 +65389,7 @@
         <v>84</v>
       </c>
       <c r="E55" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F55" s="45" t="s">
         <v>728</v>
@@ -65398,13 +65398,13 @@
         <v>638</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I55" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K55" s="25">
         <v>1.7000000000000001E-2</v>
@@ -65448,7 +65448,7 @@
         <v>83</v>
       </c>
       <c r="E56" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F56" s="45" t="s">
         <v>728</v>
@@ -65457,13 +65457,13 @@
         <v>638</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I56" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J56" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K56" s="25">
         <v>1.7000000000000001E-2</v>
@@ -65507,7 +65507,7 @@
         <v>725</v>
       </c>
       <c r="E57" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F57" s="45" t="s">
         <v>728</v>
@@ -65516,13 +65516,13 @@
         <v>642</v>
       </c>
       <c r="H57" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="J57" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K57" s="25" t="s">
         <v>26</v>
@@ -65566,7 +65566,7 @@
         <v>729</v>
       </c>
       <c r="E58" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F58" s="45" t="s">
         <v>728</v>
@@ -65575,13 +65575,13 @@
         <v>638</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I58" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J58" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K58" s="25" t="s">
         <v>26</v>
@@ -65616,10 +65616,10 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="21" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C59" s="45" t="str">
         <f t="shared" si="8"/>
@@ -65630,7 +65630,7 @@
         <v>Spodoptera_descoinsi_Spodoptera_latifascia</v>
       </c>
       <c r="E59" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F59" s="45" t="s">
         <v>730</v>
@@ -65639,13 +65639,13 @@
         <v>643</v>
       </c>
       <c r="H59" s="32" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="I59" s="32" t="s">
         <v>648</v>
       </c>
       <c r="J59" s="32" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
       <c r="K59" s="34">
         <v>4.2999999999999997E-2</v>
@@ -65694,22 +65694,22 @@
         <v>Teleogryllus_commodus_Teleogryllus_oceanicus</v>
       </c>
       <c r="E60" s="45" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F60" s="45" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G60" s="32" t="s">
         <v>666</v>
       </c>
       <c r="H60" s="32" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="I60" s="21" t="s">
         <v>647</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K60" s="34">
         <v>0.123</v>
@@ -65759,7 +65759,7 @@
         <v>65</v>
       </c>
       <c r="E61" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F61" s="45" t="s">
         <v>728</v>
@@ -65768,13 +65768,13 @@
         <v>638</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I61" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J61" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L61" s="40">
         <v>5.0999999999999997E-2</v>
@@ -65818,7 +65818,7 @@
         <v>59</v>
       </c>
       <c r="E62" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F62" s="45" t="s">
         <v>728</v>
@@ -65827,13 +65827,13 @@
         <v>638</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I62" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="L62" s="40">
         <v>5.0999999999999997E-2</v>
@@ -65877,7 +65877,7 @@
         <v>90</v>
       </c>
       <c r="E63" s="45" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="F63" s="45" t="s">
         <v>728</v>
@@ -65886,13 +65886,13 @@
         <v>638</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="I63" s="21" t="s">
         <v>646</v>
       </c>
       <c r="J63" s="21" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="K63" s="25">
         <v>1.7000000000000001E-2</v>

</xml_diff>

<commit_message>
added plot indicating how parental difference affect direction of transgression
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40BB0FA-8E99-45C2-BE1D-7288F8BEBD2E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D00A66-436B-4436-AA59-F9864AD1AC28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18480" windowHeight="11020" tabRatio="997" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62062,10 +62062,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z570"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="16.5"/>
@@ -64169,7 +64169,7 @@
         <v>688</v>
       </c>
       <c r="C34" s="45" t="str">
-        <f t="shared" ref="C34:D62" si="8">A34&amp;"_"&amp;B34</f>
+        <f t="shared" ref="C34:C62" si="8">A34&amp;"_"&amp;B34</f>
         <v>Coturnix_coturnix_coturnix_Coturnix_japonica</v>
       </c>
       <c r="D34" s="58" t="str">

</xml_diff>

<commit_message>
Combined all codes. Changed wording "TS" to novelty.
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4F7BF4-FA17-40D1-8899-452D359B6CBD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD7B9BA-8ED7-48B6-8721-DBDE8EF8F6A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18480" windowHeight="11020" tabRatio="997" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -4274,7 +4276,7 @@
   <dimension ref="A1:AS557"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D135" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G148" sqref="G148"/>
@@ -63953,10 +63955,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5C8A46-EA2B-4375-A470-1D2BA981D131}">
   <dimension ref="A1:Z570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="16.5"/>
@@ -66504,7 +66506,7 @@
         <v>623</v>
       </c>
       <c r="C41" s="45" t="str">
-        <f t="shared" si="8"/>
+        <f>A41&amp;"_"&amp;B41</f>
         <v>Haplochromis_burtoni_Haplochromis_nubilus</v>
       </c>
       <c r="D41" s="58" t="str">

</xml_diff>

<commit_message>
Deleted unused files Show credible interval in MCMCglmm analyses
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9108AD-AAB8-4CB9-AD0B-32A5957B21D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26E7B5F-CA96-49FF-904D-B126CB0729F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
-    <sheet name="Species.level.data" sheetId="6" r:id="rId2"/>
+    <sheet name="Species.level.moderators" sheetId="6" r:id="rId2"/>
     <sheet name="Description" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Phenotype!$A$1:$AM$555</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Species.level.data'!$A$1:$V$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Species.level.moderators'!$A$1:$V$62</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Phenotype!$A$1:$AM$557</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="1">'Species.level.data'!$A$1:$V$574</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'Species.level.moderators'!$A$1:$V$574</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">Phenotype!$A$1:$AM$557</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="1">'Species.level.data'!$A$1:$V$574</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">'Species.level.moderators'!$A$1:$V$574</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52492,7 +52492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5C8A46-EA2B-4375-A470-1D2BA981D131}">
   <dimension ref="A1:X570"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -69024,7 +69024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FEAB9C-4BA5-47C7-AA3E-15C9940AF475}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -69246,5 +69246,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Show credible interval in MCMCglmm analyses
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9108AD-AAB8-4CB9-AD0B-32A5957B21D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26E7B5F-CA96-49FF-904D-B126CB0729F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
-    <sheet name="Species.level.data" sheetId="6" r:id="rId2"/>
+    <sheet name="Species.level.moderators" sheetId="6" r:id="rId2"/>
     <sheet name="Description" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Phenotype!$A$1:$AM$555</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Species.level.data'!$A$1:$V$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Species.level.moderators'!$A$1:$V$62</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Phenotype!$A$1:$AM$557</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="1">'Species.level.data'!$A$1:$V$574</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'Species.level.moderators'!$A$1:$V$574</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="0">Phenotype!$A$1:$AM$557</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="1">'Species.level.data'!$A$1:$V$574</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">'Species.level.moderators'!$A$1:$V$574</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52492,7 +52492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5C8A46-EA2B-4375-A470-1D2BA981D131}">
   <dimension ref="A1:X570"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
@@ -69024,7 +69024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FEAB9C-4BA5-47C7-AA3E-15C9940AF475}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -69246,5 +69246,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reanalyse using consistent phylogenetic tree
</commit_message>
<xml_diff>
--- a/data/original.data.xlsx
+++ b/data/original.data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katsu\Desktop\Meta_F1HybridVariation.scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F305E-6105-41C5-BC79-AEF12566D976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF34CA3-EB68-4A52-9CE7-8B51823232A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" tabRatio="997" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
     <sheet name="Species.level.moderators" sheetId="6" r:id="rId2"/>
     <sheet name="Description" sheetId="7" r:id="rId3"/>
+    <sheet name="Primary.studies" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Phenotype!$A$1:$AM$555</definedName>
@@ -280,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7964" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8069" uniqueCount="720">
   <si>
     <t>Study.ID</t>
   </si>
@@ -2340,6 +2341,219 @@
   <si>
     <t>Wells_1994</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>First.author</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Blankers, T.</t>
+  </si>
+  <si>
+    <t>Phenotypic variation and covariation indicate high evolvability of acoustic communication in crickets</t>
+  </si>
+  <si>
+    <t>Journal of Evolutionary Biology</t>
+  </si>
+  <si>
+    <t>Butlin, R. K.</t>
+  </si>
+  <si>
+    <t>Genetics of behavioural and morphological differences between parapatric subspecies of *Chorthippus parallelus* (Orthoptera: Acrididae)</t>
+  </si>
+  <si>
+    <t>Biological Journal of the Linnean Society</t>
+  </si>
+  <si>
+    <t>Carson, H. L.</t>
+  </si>
+  <si>
+    <t>Change in male secondary sexual characters in artificial interspecific hybrid populations</t>
+  </si>
+  <si>
+    <t>Proceedings of the National Academy of Sciences of the United States of America</t>
+  </si>
+  <si>
+    <t>Coyne, J.A.</t>
+  </si>
+  <si>
+    <t>Genetic basis of differences in genital morphology among three sibling species of *Drosophila*</t>
+  </si>
+  <si>
+    <t>Evolution</t>
+  </si>
+  <si>
+    <t>Genetic studies of three sibling species of *Drosophila* with relationship to theories of speciation</t>
+  </si>
+  <si>
+    <t>Genetical Research</t>
+  </si>
+  <si>
+    <t>Meiotic segregation and male recombination in interspecific hybrids of *Drosophila*</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>Genetics of morphological differences and hybrid sterility between *Drosophila sechellia* and its relatives</t>
+  </si>
+  <si>
+    <t>Crapon de caprona, MD.</t>
+  </si>
+  <si>
+    <t>Interspecific fertile hybrids of haplochromine cichlidae (Teleostei) and their possible importance for speciation</t>
+  </si>
+  <si>
+    <t>Netherlands Journal of Zoology</t>
+  </si>
+  <si>
+    <t>Deregnaucourt_2010</t>
+  </si>
+  <si>
+    <t>Derégnaucourt, S.</t>
+  </si>
+  <si>
+    <t>Interspecific hybridization as a tool to understand vocal divergence: The example of crowing in quail (Genus *Coturnix*)</t>
+  </si>
+  <si>
+    <t>PLoS ONE</t>
+  </si>
+  <si>
+    <t>Doherty &amp; Gerhardt 1984</t>
+  </si>
+  <si>
+    <t>Doherty, J. A.</t>
+  </si>
+  <si>
+    <t>Acoustic communication in hybrid treefrogs: sound production by males and selective phonotaxis by females</t>
+  </si>
+  <si>
+    <t>Journal of Comparative Physiology A</t>
+  </si>
+  <si>
+    <t>Ewing, A.W.</t>
+  </si>
+  <si>
+    <t>The genetic basis of sound production in *Drosophila pseudoobscura* and *D. persimilis*</t>
+  </si>
+  <si>
+    <t>Animal Behaviour</t>
+  </si>
+  <si>
+    <t>Van Der Sluijs, I.</t>
+  </si>
+  <si>
+    <t>Female mating preference functions predict sexual selection against hybrids between sibling species of cichlid fish</t>
+  </si>
+  <si>
+    <t>Philosophical Transactions of the Royal Society B: Biological Sciences</t>
+  </si>
+  <si>
+    <t>Gadenne, C.</t>
+  </si>
+  <si>
+    <t>Development and pheromone communication systems in hybrids of *Agrotis ipsilon* and *Agrotis segetum* (Lepidoptera: Noctuidae)</t>
+  </si>
+  <si>
+    <t>Journal of Chemical Ecology</t>
+  </si>
+  <si>
+    <t>Gottsberger, B.</t>
+  </si>
+  <si>
+    <t>Behavioral sterility of hybrid males in acoustically communicating grasshoppers (Acrididae, Gomphocerinae)</t>
+  </si>
+  <si>
+    <t>Journal of Comparative Physiology A: Neuroethology, Sensory, Neural, and Behavioral Physiology</t>
+  </si>
+  <si>
+    <t>Bentley, D. R.</t>
+  </si>
+  <si>
+    <t>Genetic control of the neuronal network generating cricket (*Teleogryllus gryllus*) song patterns</t>
+  </si>
+  <si>
+    <t>Magalhaes, I. S.</t>
+  </si>
+  <si>
+    <t>Genetics of male nuptial colour divergence between sympatric sister species of a Lake Victoria cichlid fish</t>
+  </si>
+  <si>
+    <t>Monti, L</t>
+  </si>
+  <si>
+    <t>Elliptic fourier analysis of the form of genitalia in two *Spodoptera* species and their hybrids (Lepidoptera: Noctuidae)</t>
+  </si>
+  <si>
+    <t>Musolf, K</t>
+  </si>
+  <si>
+    <t>Ultrasonic vocalizations of male mice differ among species and females show assortative preferences for male calls</t>
+  </si>
+  <si>
+    <t>Paallysaho et al_2003</t>
+  </si>
+  <si>
+    <t>Päällysaho, S.</t>
+  </si>
+  <si>
+    <t>Role of X chromosomal song genes in the evolution of species-specific courtship songs in *Drosophila virilis* group species</t>
+  </si>
+  <si>
+    <t>Behavior Genetics</t>
+  </si>
+  <si>
+    <t>Shaw, K. L.</t>
+  </si>
+  <si>
+    <t>Polygenic inheritance of a behavioral phenotype: Interspecific genetics of song in the Hawaiian cricket genus *Laupala*</t>
+  </si>
+  <si>
+    <t>Suvanto, L.</t>
+  </si>
+  <si>
+    <t>Secondary courtship songs and inhibitory songs of *Drosophila virilis*-group males</t>
+  </si>
+  <si>
+    <t>Tomaru, M.</t>
+  </si>
+  <si>
+    <t>Differences in courtship song in the species of the *Drosophila auraria* complex</t>
+  </si>
+  <si>
+    <t>Wells_1994</t>
+  </si>
+  <si>
+    <t>Wells, M. M.</t>
+  </si>
+  <si>
+    <t>Behavioral responses of hybrid lacewings (Neuroptera: Chrysopidae) to courtship songs</t>
+  </si>
+  <si>
+    <t>Journal of Insect Behavior</t>
+  </si>
+  <si>
+    <t>Interspecific genetics of mate recognition: Inheritance of female acoustic preference in Hawaiian crickets</t>
+  </si>
+  <si>
+    <t>Sasabe_et.al_2007</t>
+  </si>
+  <si>
+    <t>Sasabe, M.</t>
+  </si>
+  <si>
+    <t>The genetic basis of interspecific differences in genital morphology of closely related carabid beetles</t>
+  </si>
+  <si>
+    <t>Heredity</t>
   </si>
 </sst>
 </file>
@@ -3062,7 +3276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM557"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E535" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -69249,4 +69463,463 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B124749-DE41-4E35-A21A-2B9F13496A95}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1988</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1983</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1985</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1986</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1991</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1969</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2008</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1997</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1972</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2001</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1996</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1994</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>719</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>